<commit_message>
Added code to receive JSON linkages from unmodeled compartments for Toxicant in water. Completed complex test case for Chemical.cs. Updated programmers log and testing materials.
</commit_message>
<xml_diff>
--- a/Chemicals/TEST/P_Pond_MN_Chlorpyrifos_Simple_Wind.xlsx
+++ b/Chemicals/TEST/P_Pond_MN_Chlorpyrifos_Simple_Wind.xlsx
@@ -2681,298 +2681,6 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$BD$2:$BD$97</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="96"/>
-                <c:pt idx="0">
-                  <c:v>1.0000001028857011</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0001538997173096</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0003005743739704</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0002870919242355</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0002737039404157</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0002605757719962</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0002471529195802</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0002339790463586</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0002208772873866</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0002076339653181</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.0001944479670515</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.0001812535047898</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.0001679464067077</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.0001548312525852</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.0001417252078006</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.0001286302904768</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.0001155092359104</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.0001025079783477</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.0000892880905319</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.0000763608168879</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.0000633089110313</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.0000501201086576</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.000037185625442</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.0000239702429248</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.0000110070860448</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.99999790326279669</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.99998489069450214</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.9999717185123228</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.9999587606698549</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.99994568673683504</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.9999325696130047</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.99991944257134358</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.99990652145751657</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.99989331596044084</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.9998801848190193</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.9998672257753134</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.99985405105819758</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.99984090202535625</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.9998277580427084</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.99981455899041327</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.999801429829976</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.99978823203882383</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.99977501261351942</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.99976177994197379</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.9997485035974244</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.9997353414936504</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.9997219585007856</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.99970866333395603</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.99969527111116052</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.99968201667420054</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.99966863811752438</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.99965506381714753</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.99964164818602408</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.99962824657600513</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.99961467491417189</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.99960117925387648</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.99958750050717926</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.99957404962963314</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.999560255858294</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.99954669767992321</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.99953296710141581</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.99951909547501683</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.99950532165302519</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.9994913664256655</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.9994773999273715</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.99946356108669798</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.99944946215205099</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.99943541981388284</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.99942147361530098</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.99940737869420004</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.99939310470745391</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.99937884272327127</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.99936449950866479</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.9993502056821042</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.99933580365366004</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.9993213620954644</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.9993069206707812</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.99929222435394593</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.99927778262844713</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.9992630133075705</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.99924810158444421</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.99923348280135316</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.99921847592326229</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.99920346129421456</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.99918852436355787</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.99917344464926861</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.99915825277862313</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.99914324178601699</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.99912782163274261</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.99911252508960191</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.99909729095118505</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.99908173541505729</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.99906603806677496</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.99905066622071881</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.99903486070452574</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.99951096826256336</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -3303,11 +3011,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103540992"/>
-        <c:axId val="65671168"/>
+        <c:axId val="169489152"/>
+        <c:axId val="169490688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103540992"/>
+        <c:axId val="169489152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3316,7 +3024,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65671168"/>
+        <c:crossAx val="169490688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3324,11 +3032,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65671168"/>
+        <c:axId val="169490688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.01"/>
-          <c:min val="0.99"/>
+          <c:max val="1.02"/>
+          <c:min val="0.98"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3337,7 +3045,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103540992"/>
+        <c:crossAx val="169489152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4021,11 +3729,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="65721472"/>
-        <c:axId val="65723008"/>
+        <c:axId val="171729280"/>
+        <c:axId val="171730816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="65721472"/>
+        <c:axId val="171729280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4034,7 +3742,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65723008"/>
+        <c:crossAx val="171730816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4042,7 +3750,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65723008"/>
+        <c:axId val="171730816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4053,7 +3761,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65721472"/>
+        <c:crossAx val="171729280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4737,11 +4445,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="88114688"/>
-        <c:axId val="88116608"/>
+        <c:axId val="175337472"/>
+        <c:axId val="175339776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88114688"/>
+        <c:axId val="175337472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4750,7 +4458,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88116608"/>
+        <c:crossAx val="175339776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4758,7 +4466,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88116608"/>
+        <c:axId val="175339776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4769,7 +4477,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88114688"/>
+        <c:crossAx val="175337472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4796,13 +4504,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>39</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>71436</xdr:rowOff>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>60</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
@@ -5176,10 +4884,10 @@
   <dimension ref="A1:BE97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BI9" sqref="BI9"/>
+      <selection pane="bottomRight" activeCell="AT46" sqref="AT46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5205,7 +4913,7 @@
     <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="0" hidden="1" customWidth="1"/>
     <col min="47" max="52" width="0" hidden="1" customWidth="1"/>
-    <col min="54" max="55" width="0" hidden="1" customWidth="1"/>
+    <col min="54" max="56" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57" x14ac:dyDescent="0.25">

</xml_diff>